<commit_message>
CreateEntryExit adapted to no sterility records, uses start/end spell dates, removes recs exit < entry/CPRD proc code correction/days to years calc correction (createbaseline)
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
+++ b/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31653\Desktop\LOT4_SmartGit\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31653\Desktop\LOT4_Sourcetree\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9016C822-6B68-48C1-9D48-929957EA9487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAAA763-907F-4F12-A7DB-B9C8E80CA455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,9 +353,6 @@
     <t>Coding System</t>
   </si>
   <si>
-    <t>OPCS</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description </t>
   </si>
   <si>
@@ -822,6 +819,9 @@
   </si>
   <si>
     <t xml:space="preserve">unspecified other endoscopic occlusion of fallopian tube </t>
+  </si>
+  <si>
+    <t>OPCS4</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,13 +1244,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -1266,13 +1266,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -1288,13 +1288,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -1310,13 +1310,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -1354,13 +1354,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>49</v>
@@ -1398,13 +1398,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>49</v>
@@ -1420,13 +1420,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>49</v>
@@ -1442,13 +1442,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
@@ -1464,13 +1464,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>49</v>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>49</v>
@@ -1552,13 +1552,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>49</v>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20DF1C-1822-48BD-A5E8-6C607BCB50D4}">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="13">
         <v>5682</v>
@@ -1768,12 +1768,12 @@
         <v>54</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="13">
         <v>5682</v>
@@ -1782,12 +1782,12 @@
         <v>54</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="13">
         <v>5683</v>
@@ -1796,12 +1796,12 @@
         <v>54</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" s="13">
         <v>5684</v>
@@ -1810,12 +1810,12 @@
         <v>54</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="13">
         <v>5685</v>
@@ -1824,12 +1824,12 @@
         <v>54</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="13">
         <v>5686</v>
@@ -1838,12 +1838,12 @@
         <v>54</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="13">
         <v>5687</v>
@@ -1852,12 +1852,12 @@
         <v>54</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13">
         <v>5688</v>
@@ -1866,12 +1866,12 @@
         <v>54</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="13">
         <v>37051</v>
@@ -1880,12 +1880,12 @@
         <v>63</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B11" s="13">
         <v>37051</v>
@@ -1894,12 +1894,12 @@
         <v>98</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" s="13">
         <v>37052</v>
@@ -1908,12 +1908,12 @@
         <v>63</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" s="13">
         <v>37052</v>
@@ -1922,12 +1922,12 @@
         <v>98</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="13">
         <v>37131</v>
@@ -1936,12 +1936,12 @@
         <v>63</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="13">
         <v>37131</v>
@@ -1950,12 +1950,12 @@
         <v>98</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B16" s="13">
         <v>37132</v>
@@ -1964,12 +1964,12 @@
         <v>63</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B17" s="13">
         <v>37140</v>
@@ -1978,12 +1978,12 @@
         <v>63</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" s="13">
         <v>37171</v>
@@ -1992,12 +1992,12 @@
         <v>63</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" s="13">
         <v>37171</v>
@@ -2006,12 +2006,12 @@
         <v>98</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B20" s="13">
         <v>37172</v>
@@ -2020,12 +2020,12 @@
         <v>63</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" s="13">
         <v>37172</v>
@@ -2034,12 +2034,12 @@
         <v>98</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="13">
         <v>56820</v>
@@ -2048,12 +2048,12 @@
         <v>54</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="13">
         <v>56828</v>
@@ -2062,12 +2062,12 @@
         <v>54</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="13">
         <v>56829</v>
@@ -2076,12 +2076,12 @@
         <v>54</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="13">
         <v>56830</v>
@@ -2090,12 +2090,12 @@
         <v>54</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="13">
         <v>56831</v>
@@ -2104,12 +2104,12 @@
         <v>54</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="13">
         <v>56832</v>
@@ -2118,12 +2118,12 @@
         <v>54</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="13">
         <v>56833</v>
@@ -2132,12 +2132,12 @@
         <v>54</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="13">
         <v>56838</v>
@@ -2146,12 +2146,12 @@
         <v>54</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="13">
         <v>56839</v>
@@ -2160,12 +2160,12 @@
         <v>54</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="13">
         <v>56840</v>
@@ -2174,12 +2174,12 @@
         <v>54</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="13">
         <v>56841</v>
@@ -2188,12 +2188,12 @@
         <v>54</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="13">
         <v>56842</v>
@@ -2202,12 +2202,12 @@
         <v>54</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="13">
         <v>56843</v>
@@ -2216,12 +2216,12 @@
         <v>54</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="13">
         <v>56848</v>
@@ -2230,12 +2230,12 @@
         <v>54</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="13">
         <v>56849</v>
@@ -2244,7 +2244,7 @@
         <v>54</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B37" s="13">
         <v>56850</v>
@@ -2261,7 +2261,7 @@
         <v>54</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H37"/>
       <c r="I37"/>
@@ -2269,7 +2269,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B38" s="13">
         <v>56851</v>
@@ -2278,7 +2278,7 @@
         <v>54</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="13">
         <v>56852</v>
@@ -2295,7 +2295,7 @@
         <v>54</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H39"/>
       <c r="I39"/>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B40" s="13">
         <v>56853</v>
@@ -2312,7 +2312,7 @@
         <v>54</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40"/>
       <c r="I40"/>
@@ -2320,7 +2320,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="13">
         <v>56859</v>
@@ -2329,7 +2329,7 @@
         <v>54</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H41"/>
       <c r="I41"/>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="13">
         <v>56860</v>
@@ -2346,7 +2346,7 @@
         <v>54</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H42"/>
       <c r="I42"/>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="13">
         <v>56861</v>
@@ -2363,7 +2363,7 @@
         <v>54</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H43"/>
       <c r="I43"/>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" s="13">
         <v>56862</v>
@@ -2380,7 +2380,7 @@
         <v>54</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H44"/>
       <c r="I44"/>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45" s="13">
         <v>56869</v>
@@ -2397,7 +2397,7 @@
         <v>54</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H45"/>
       <c r="I45"/>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" s="13">
         <v>56870</v>
@@ -2414,7 +2414,7 @@
         <v>54</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H46"/>
       <c r="I46"/>
@@ -2422,7 +2422,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="13">
         <v>56871</v>
@@ -2431,7 +2431,7 @@
         <v>54</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H47"/>
       <c r="I47"/>
@@ -2439,7 +2439,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="13">
         <v>56872</v>
@@ -2448,7 +2448,7 @@
         <v>54</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H48"/>
       <c r="I48"/>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" s="13">
         <v>56879</v>
@@ -2465,7 +2465,7 @@
         <v>54</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H49"/>
       <c r="I49"/>
@@ -2473,7 +2473,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" s="13">
         <v>57034</v>
@@ -2482,7 +2482,7 @@
         <v>54</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H50"/>
       <c r="I50"/>
@@ -2490,7 +2490,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B51" s="13">
         <v>197011</v>
@@ -2499,7 +2499,7 @@
         <v>63</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H51"/>
       <c r="I51"/>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B52" s="13">
         <v>197011</v>
@@ -2516,7 +2516,7 @@
         <v>98</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H52"/>
       <c r="I52"/>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B53" s="13">
         <v>199906</v>
@@ -2533,7 +2533,7 @@
         <v>63</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H53"/>
       <c r="I53"/>
@@ -2541,7 +2541,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B54" s="13">
         <v>199906</v>
@@ -2550,7 +2550,7 @@
         <v>63</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H54"/>
       <c r="I54"/>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B55" s="13">
         <v>199906</v>
@@ -2567,7 +2567,7 @@
         <v>98</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H55"/>
       <c r="I55"/>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B56" s="13">
         <v>199906</v>
@@ -2584,7 +2584,7 @@
         <v>98</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H56"/>
       <c r="I56"/>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B57" s="13">
         <v>199907</v>
@@ -2601,7 +2601,7 @@
         <v>63</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H57"/>
       <c r="I57"/>
@@ -2609,7 +2609,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" s="13">
         <v>199907</v>
@@ -2618,7 +2618,7 @@
         <v>63</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H58"/>
       <c r="I58"/>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" s="13">
         <v>199907</v>
@@ -2635,7 +2635,7 @@
         <v>98</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H59"/>
       <c r="I59"/>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" s="13">
         <v>199907</v>
@@ -2652,7 +2652,7 @@
         <v>98</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
@@ -2660,7 +2660,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B61" s="13">
         <v>337052</v>
@@ -2669,7 +2669,7 @@
         <v>63</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B62" s="13">
         <v>337058</v>
@@ -2686,7 +2686,7 @@
         <v>63</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H62"/>
       <c r="I62"/>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B63" s="13">
         <v>337059</v>
@@ -2703,7 +2703,7 @@
         <v>63</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
@@ -2720,7 +2720,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H64"/>
       <c r="I64"/>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B65" s="13">
         <v>568280</v>
@@ -2737,7 +2737,7 @@
         <v>54</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H65"/>
       <c r="I65"/>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B66" s="13">
         <v>568281</v>
@@ -2754,7 +2754,7 @@
         <v>54</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H66"/>
       <c r="I66"/>
@@ -2762,7 +2762,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" s="13">
         <v>568282</v>
@@ -2771,7 +2771,7 @@
         <v>54</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H67"/>
       <c r="I67"/>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="13">
         <v>687217</v>
@@ -2788,7 +2788,7 @@
         <v>63</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H68"/>
       <c r="I68"/>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B69" s="13">
         <v>687218</v>
@@ -2805,7 +2805,7 @@
         <v>63</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H69"/>
       <c r="I69"/>
@@ -2813,7 +2813,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="13">
         <v>687219</v>
@@ -2822,7 +2822,7 @@
         <v>63</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H70"/>
       <c r="I70"/>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B71" s="13">
         <v>687219</v>
@@ -2839,7 +2839,7 @@
         <v>63</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H71"/>
       <c r="I71"/>
@@ -2847,16 +2847,16 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H72"/>
       <c r="I72"/>
@@ -2864,16 +2864,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H73"/>
       <c r="I73"/>
@@ -2881,16 +2881,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H74"/>
       <c r="I74"/>
@@ -2898,16 +2898,16 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H75"/>
       <c r="I75"/>
@@ -2915,16 +2915,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H76"/>
       <c r="I76"/>
@@ -2932,16 +2932,16 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H77"/>
       <c r="I77"/>
@@ -2949,16 +2949,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H78"/>
       <c r="I78"/>
@@ -2966,16 +2966,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H79"/>
       <c r="I79"/>
@@ -2983,16 +2983,16 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H80"/>
       <c r="I80"/>
@@ -3000,16 +3000,16 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H81"/>
       <c r="I81"/>
@@ -3017,16 +3017,16 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>63</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H82"/>
       <c r="I82"/>
@@ -3034,13 +3034,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>50</v>
@@ -3051,13 +3051,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B84" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>50</v>
@@ -3068,13 +3068,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>50</v>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B86" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>50</v>
@@ -3102,13 +3102,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B87" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D87" s="12" t="s">
         <v>50</v>
@@ -3119,13 +3119,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>50</v>
@@ -3136,13 +3136,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B89" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D89" s="12" t="s">
         <v>50</v>
@@ -3153,13 +3153,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B90" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D90" s="12" t="s">
         <v>50</v>
@@ -3170,13 +3170,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B91" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>50</v>
@@ -3187,13 +3187,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="14" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>50</v>
@@ -3204,13 +3204,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>50</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B94" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>50</v>
@@ -3238,13 +3238,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>50</v>
@@ -3255,13 +3255,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>50</v>
@@ -3272,13 +3272,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>50</v>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>50</v>
@@ -3306,13 +3306,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D99" s="12" t="s">
         <v>50</v>
@@ -3323,13 +3323,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D100" s="12" t="s">
         <v>50</v>
@@ -3340,13 +3340,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D101" s="12" t="s">
         <v>50</v>
@@ -3357,13 +3357,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D102" s="12" t="s">
         <v>50</v>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B103" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D103" s="12" t="s">
         <v>50</v>
@@ -3391,13 +3391,13 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B104" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D104" s="12" t="s">
         <v>50</v>
@@ -3408,13 +3408,13 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D105" s="12" t="s">
         <v>50</v>
@@ -3425,13 +3425,13 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D106" s="12" t="s">
         <v>50</v>
@@ -3442,13 +3442,13 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D107" s="12" t="s">
         <v>50</v>
@@ -3459,13 +3459,13 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B108" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D108" s="12" t="s">
         <v>50</v>
@@ -3476,13 +3476,13 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D109" s="12" t="s">
         <v>50</v>
@@ -3493,13 +3493,13 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B110" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D110" s="12" t="s">
         <v>50</v>
@@ -3510,13 +3510,13 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B111" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D111" s="12" t="s">
         <v>50</v>
@@ -3527,13 +3527,13 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>50</v>
@@ -3544,13 +3544,13 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B113" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>50</v>
@@ -3561,13 +3561,13 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D114" s="12" t="s">
         <v>50</v>
@@ -3578,13 +3578,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B115" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>102</v>
+        <v>258</v>
       </c>
       <c r="D115" s="12" t="s">
         <v>50</v>
@@ -3615,7 +3615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E766E548-8393-46AC-AB7C-3B6B1ADADF6D}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -3630,7 +3630,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>51</v>
@@ -3653,7 +3653,7 @@
         <v>54</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,7 +3667,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>54</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,7 +3695,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3709,7 +3709,7 @@
         <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3723,7 +3723,7 @@
         <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3737,7 +3737,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3751,7 +3751,7 @@
         <v>54</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3765,7 +3765,7 @@
         <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3779,7 +3779,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3793,7 +3793,7 @@
         <v>63</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,7 +3807,7 @@
         <v>63</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3821,7 +3821,7 @@
         <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,7 +3835,7 @@
         <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3863,7 +3863,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>63</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3891,7 +3891,7 @@
         <v>63</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,7 +3905,7 @@
         <v>63</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3919,7 +3919,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
         <v>63</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3947,7 +3947,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,7 +3961,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
         <v>63</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
         <v>63</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4003,7 +4003,7 @@
         <v>63</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4017,7 +4017,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4031,7 +4031,7 @@
         <v>63</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
         <v>63</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4059,7 +4059,7 @@
         <v>63</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4073,7 +4073,7 @@
         <v>63</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4087,7 +4087,7 @@
         <v>63</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,7 +4101,7 @@
         <v>63</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,7 +4115,7 @@
         <v>63</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4129,7 +4129,7 @@
         <v>63</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
         <v>63</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4157,7 +4157,7 @@
         <v>63</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>63</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4185,7 +4185,7 @@
         <v>98</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4199,7 +4199,7 @@
         <v>98</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4213,7 +4213,7 @@
         <v>98</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4227,7 +4227,7 @@
         <v>98</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4241,7 +4241,7 @@
         <v>98</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="6">
         <v>370804</v>
@@ -4288,12 +4288,12 @@
         <v>63</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="6">
         <v>197006</v>
@@ -4302,12 +4302,12 @@
         <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="6">
         <v>370803</v>
@@ -4316,12 +4316,12 @@
         <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="6">
         <v>78041</v>
@@ -4330,12 +4330,12 @@
         <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="6">
         <v>78081</v>
@@ -4344,12 +4344,12 @@
         <v>63</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7" s="6">
         <v>72557</v>
@@ -4358,12 +4358,12 @@
         <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="6">
         <v>72558</v>
@@ -4372,12 +4372,12 @@
         <v>63</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="6">
         <v>72559</v>
@@ -4386,432 +4386,432 @@
         <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B40" s="6">
         <v>376479</v>
@@ -4820,12 +4820,12 @@
         <v>63</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B41" s="6">
         <v>376479</v>
@@ -4834,12 +4834,12 @@
         <v>63</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B42" s="6">
         <v>376479</v>
@@ -4848,12 +4848,12 @@
         <v>63</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B43" s="6">
         <v>197006</v>
@@ -4862,12 +4862,12 @@
         <v>98</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B44" s="6">
         <v>78041</v>
@@ -4876,12 +4876,12 @@
         <v>98</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B45" s="6">
         <v>78081</v>
@@ -4890,12 +4890,12 @@
         <v>98</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B46" s="6">
         <v>72557</v>
@@ -4904,12 +4904,12 @@
         <v>98</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B47" s="6">
         <v>72558</v>
@@ -4918,12 +4918,12 @@
         <v>98</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B48" s="6">
         <v>72559</v>
@@ -4932,7 +4932,7 @@
         <v>98</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction of PHARMO cordelists
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
+++ b/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31653\Desktop\LOT4_Sourcetree\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAAA763-907F-4F12-A7DB-B9C8E80CA455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16967E0C-5241-4D84-9AD8-F8895B0DF88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hysterectomy" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="260">
   <si>
     <t>Q07</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Vaginaal verwijderen en inbrengen van intra-uterien corpus alienum</t>
   </si>
   <si>
-    <t>CVV</t>
-  </si>
-  <si>
     <t>Vaginale verwijdering van intra-uterien corpus alienum</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>I.U.D. KOPERHOUDEND         MULTI LOAD - SHORT</t>
   </si>
   <si>
-    <t>CBV</t>
-  </si>
-  <si>
     <t>I.U.D. KOPERHOUDEND         MULTI LOAD</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>ABORTUSKLINIEK - SPIRAALTJE VERWIJDEREN</t>
   </si>
   <si>
-    <t>ZA</t>
-  </si>
-  <si>
     <t>UTERUS - PLAATSEN SPIRAAL --I.U.D. OF I.U.S.--</t>
   </si>
   <si>
@@ -822,6 +813,18 @@
   </si>
   <si>
     <t>OPCS4</t>
+  </si>
+  <si>
+    <t>cvv_procedure</t>
+  </si>
+  <si>
+    <t>cbv_procedure</t>
+  </si>
+  <si>
+    <t>za_procedure</t>
+  </si>
+  <si>
+    <t>za_procedure_procedure</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B917A76D-CD72-406A-B576-3D4A2F81E0E4}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1216,19 +1219,19 @@
   <cols>
     <col min="1" max="1" width="55.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>52</v>
@@ -1244,13 +1247,13 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -1266,13 +1269,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -1288,13 +1291,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -1310,13 +1313,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
@@ -1332,13 +1335,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -1354,13 +1357,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
@@ -1376,13 +1379,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>49</v>
@@ -1398,13 +1401,13 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>49</v>
@@ -1420,13 +1423,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>49</v>
@@ -1442,13 +1445,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
@@ -1464,13 +1467,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>49</v>
@@ -1486,13 +1489,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -1508,13 +1511,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -1530,13 +1533,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>49</v>
@@ -1552,13 +1555,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>49</v>
@@ -1574,13 +1577,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
@@ -1730,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20DF1C-1822-48BD-A5E8-6C607BCB50D4}">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,13 +1748,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>52</v>
@@ -1759,492 +1762,492 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2" s="13">
         <v>5682</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3" s="13">
         <v>5682</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" s="13">
         <v>5683</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B5" s="13">
         <v>5684</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" s="13">
         <v>5685</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B7" s="13">
         <v>5686</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B8" s="13">
         <v>5687</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B9" s="13">
         <v>5688</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B10" s="13">
         <v>37051</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" s="13">
         <v>37051</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B12" s="13">
         <v>37052</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B13" s="13">
         <v>37052</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B14" s="13">
         <v>37131</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B15" s="13">
         <v>37131</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B16" s="13">
         <v>37132</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B17" s="13">
         <v>37140</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B18" s="13">
         <v>37171</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B19" s="13">
         <v>37171</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B20" s="13">
         <v>37172</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="13">
         <v>37172</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B22" s="13">
         <v>56820</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B23" s="13">
         <v>56828</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B24" s="13">
         <v>56829</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B25" s="13">
         <v>56830</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B26" s="13">
         <v>56831</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B27" s="13">
         <v>56832</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B28" s="13">
         <v>56833</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B29" s="13">
         <v>56838</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B30" s="13">
         <v>56839</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B31" s="13">
         <v>56840</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B32" s="13">
         <v>56841</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B33" s="13">
         <v>56842</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B34" s="13">
         <v>56843</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B35" s="13">
         <v>56848</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B36" s="13">
         <v>56849</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H36"/>
       <c r="I36"/>
@@ -2252,16 +2255,16 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B37" s="13">
         <v>56850</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H37"/>
       <c r="I37"/>
@@ -2269,16 +2272,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B38" s="13">
         <v>56851</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H38"/>
       <c r="I38"/>
@@ -2286,16 +2289,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B39" s="13">
         <v>56852</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H39"/>
       <c r="I39"/>
@@ -2303,16 +2306,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B40" s="13">
         <v>56853</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H40"/>
       <c r="I40"/>
@@ -2320,16 +2323,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B41" s="13">
         <v>56859</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H41"/>
       <c r="I41"/>
@@ -2337,16 +2340,16 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B42" s="13">
         <v>56860</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H42"/>
       <c r="I42"/>
@@ -2354,16 +2357,16 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B43" s="13">
         <v>56861</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H43"/>
       <c r="I43"/>
@@ -2371,16 +2374,16 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B44" s="13">
         <v>56862</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H44"/>
       <c r="I44"/>
@@ -2388,16 +2391,16 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B45" s="13">
         <v>56869</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H45"/>
       <c r="I45"/>
@@ -2405,16 +2408,16 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B46" s="13">
         <v>56870</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H46"/>
       <c r="I46"/>
@@ -2422,16 +2425,16 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B47" s="13">
         <v>56871</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H47"/>
       <c r="I47"/>
@@ -2439,16 +2442,16 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B48" s="13">
         <v>56872</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H48"/>
       <c r="I48"/>
@@ -2456,16 +2459,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B49" s="13">
         <v>56879</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H49"/>
       <c r="I49"/>
@@ -2473,16 +2476,16 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B50" s="13">
         <v>57034</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H50"/>
       <c r="I50"/>
@@ -2490,16 +2493,16 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B51" s="13">
         <v>197011</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H51"/>
       <c r="I51"/>
@@ -2507,16 +2510,16 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B52" s="13">
         <v>197011</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H52"/>
       <c r="I52"/>
@@ -2524,16 +2527,16 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B53" s="13">
         <v>199906</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H53"/>
       <c r="I53"/>
@@ -2541,16 +2544,16 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B54" s="13">
         <v>199906</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H54"/>
       <c r="I54"/>
@@ -2558,16 +2561,16 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B55" s="13">
         <v>199906</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H55"/>
       <c r="I55"/>
@@ -2575,16 +2578,16 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B56" s="13">
         <v>199906</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H56"/>
       <c r="I56"/>
@@ -2592,16 +2595,16 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B57" s="13">
         <v>199907</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H57"/>
       <c r="I57"/>
@@ -2609,16 +2612,16 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B58" s="13">
         <v>199907</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H58"/>
       <c r="I58"/>
@@ -2626,16 +2629,16 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B59" s="13">
         <v>199907</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H59"/>
       <c r="I59"/>
@@ -2643,16 +2646,16 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B60" s="13">
         <v>199907</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
@@ -2660,16 +2663,16 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B61" s="13">
         <v>337052</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
@@ -2677,16 +2680,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B62" s="13">
         <v>337058</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H62"/>
       <c r="I62"/>
@@ -2694,16 +2697,16 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B63" s="13">
         <v>337059</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
@@ -2711,16 +2714,16 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B64" s="13">
         <v>337293</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H64"/>
       <c r="I64"/>
@@ -2728,16 +2731,16 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B65" s="13">
         <v>568280</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H65"/>
       <c r="I65"/>
@@ -2745,16 +2748,16 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B66" s="13">
         <v>568281</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H66"/>
       <c r="I66"/>
@@ -2762,16 +2765,16 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B67" s="13">
         <v>568282</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H67"/>
       <c r="I67"/>
@@ -2779,16 +2782,16 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B68" s="13">
         <v>687217</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H68"/>
       <c r="I68"/>
@@ -2796,16 +2799,16 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B69" s="13">
         <v>687218</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H69"/>
       <c r="I69"/>
@@ -2813,16 +2816,16 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B70" s="13">
         <v>687219</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H70"/>
       <c r="I70"/>
@@ -2830,16 +2833,16 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B71" s="13">
         <v>687219</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H71"/>
       <c r="I71"/>
@@ -2847,16 +2850,16 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H72"/>
       <c r="I72"/>
@@ -2864,16 +2867,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H73"/>
       <c r="I73"/>
@@ -2881,16 +2884,16 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H74"/>
       <c r="I74"/>
@@ -2898,16 +2901,16 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H75"/>
       <c r="I75"/>
@@ -2915,16 +2918,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H76"/>
       <c r="I76"/>
@@ -2932,16 +2935,16 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H77"/>
       <c r="I77"/>
@@ -2949,16 +2952,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H78"/>
       <c r="I78"/>
@@ -2966,16 +2969,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H79"/>
       <c r="I79"/>
@@ -2983,16 +2986,16 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H80"/>
       <c r="I80"/>
@@ -3000,16 +3003,16 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H81"/>
       <c r="I81"/>
@@ -3017,16 +3020,16 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H82"/>
       <c r="I82"/>
@@ -3034,13 +3037,13 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B83" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C83" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>50</v>
@@ -3051,13 +3054,13 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B84" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>50</v>
@@ -3068,13 +3071,13 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="14" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>50</v>
@@ -3085,13 +3088,13 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B86" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>50</v>
@@ -3102,13 +3105,13 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B87" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D87" s="12" t="s">
         <v>50</v>
@@ -3119,13 +3122,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="14" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>50</v>
@@ -3136,13 +3139,13 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="14" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B89" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D89" s="12" t="s">
         <v>50</v>
@@ -3153,13 +3156,13 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B90" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D90" s="12" t="s">
         <v>50</v>
@@ -3170,13 +3173,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="14" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B91" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>50</v>
@@ -3187,13 +3190,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B92" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>50</v>
@@ -3204,13 +3207,13 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B93" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>50</v>
@@ -3221,13 +3224,13 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B94" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>50</v>
@@ -3238,13 +3241,13 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>50</v>
@@ -3255,13 +3258,13 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B96" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>50</v>
@@ -3272,13 +3275,13 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B97" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>50</v>
@@ -3289,13 +3292,13 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>50</v>
@@ -3306,13 +3309,13 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D99" s="12" t="s">
         <v>50</v>
@@ -3323,13 +3326,13 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B100" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D100" s="12" t="s">
         <v>50</v>
@@ -3340,13 +3343,13 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D101" s="12" t="s">
         <v>50</v>
@@ -3357,13 +3360,13 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="14" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B102" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D102" s="12" t="s">
         <v>50</v>
@@ -3374,13 +3377,13 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B103" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D103" s="12" t="s">
         <v>50</v>
@@ -3391,13 +3394,13 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B104" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D104" s="12" t="s">
         <v>50</v>
@@ -3408,13 +3411,13 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B105" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D105" s="12" t="s">
         <v>50</v>
@@ -3425,13 +3428,13 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B106" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D106" s="12" t="s">
         <v>50</v>
@@ -3442,13 +3445,13 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B107" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D107" s="12" t="s">
         <v>50</v>
@@ -3459,13 +3462,13 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="14" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B108" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D108" s="12" t="s">
         <v>50</v>
@@ -3476,13 +3479,13 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B109" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D109" s="12" t="s">
         <v>50</v>
@@ -3493,13 +3496,13 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B110" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D110" s="12" t="s">
         <v>50</v>
@@ -3510,13 +3513,13 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B111" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D111" s="12" t="s">
         <v>50</v>
@@ -3527,13 +3530,13 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B112" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>50</v>
@@ -3544,13 +3547,13 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B113" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>50</v>
@@ -3561,13 +3564,13 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B114" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D114" s="12" t="s">
         <v>50</v>
@@ -3578,13 +3581,13 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B115" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D115" s="12" t="s">
         <v>50</v>
@@ -3623,20 +3626,20 @@
   <cols>
     <col min="1" max="1" width="62.88671875" style="6" customWidth="1"/>
     <col min="2" max="2" width="10.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>52</v>
@@ -3650,598 +3653,598 @@
         <v>5691</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="19">
         <v>5691</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="19">
         <v>56911</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="19">
         <v>4653</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="19">
         <v>56910</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="19">
         <v>569100</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="19">
         <v>569101</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19">
         <v>569102</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="20">
         <v>687199</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="20">
         <v>687200</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="20">
         <v>687201</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="20">
         <v>687202</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="20">
         <v>687203</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="20">
         <v>687204</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="20">
         <v>687205</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="20">
         <v>687206</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="20">
         <v>687210</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="20">
         <v>687211</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="20">
         <v>687212</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="20">
         <v>687213</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="20">
         <v>687214</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="20">
         <v>687215</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="20">
         <v>37180</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="20">
         <v>197008</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" s="20">
         <v>727940</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B27" s="20">
         <v>190274</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="20">
         <v>337292</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B31" s="20">
         <v>337293</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B32" s="20">
         <v>337295</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B38" s="20">
         <v>37173</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" s="20">
         <v>197009</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" s="20">
         <v>37180</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B41" s="20">
         <v>37180</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" s="20">
         <v>197008</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B43" s="20">
         <v>197009</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="20">
         <v>190274</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4253,25 +4256,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38C000B-F835-4075-843C-2308CB7B2E7C}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A12"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.5546875" style="6" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="8.88671875" style="6"/>
+    <col min="3" max="3" width="60.44140625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>52</v>
@@ -4279,660 +4284,660 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B2" s="6">
         <v>370804</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B3" s="6">
         <v>197006</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B4" s="6">
         <v>370803</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B5" s="6">
         <v>78041</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B6" s="6">
         <v>78081</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B7" s="6">
         <v>72557</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B8" s="6">
         <v>72558</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B9" s="6">
         <v>72559</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B40" s="6">
         <v>376479</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B41" s="6">
         <v>376479</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B42" s="6">
         <v>376479</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B43" s="6">
         <v>197006</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B44" s="6">
         <v>78041</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B45" s="6">
         <v>78081</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B46" s="6">
         <v>72557</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B47" s="6">
         <v>72558</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B48" s="6">
         <v>72559</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
procedure code syntax correction
</commit_message>
<xml_diff>
--- a/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
+++ b/DEVELOPMENT/LOT4_scripts/p_steps/CodeLists/Procedure_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31653\Desktop\LOT4_Sourcetree\DEVELOPMENT\LOT4_scripts\p_steps\CodeLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AE3893-C4C5-42E1-88B6-FC60E9AD4CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02DE01A-4BC3-41C7-9681-00DF7531B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sterilisation" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="259">
   <si>
     <t>Q07</t>
   </si>
@@ -821,9 +821,6 @@
   </si>
   <si>
     <t>za_procedure</t>
-  </si>
-  <si>
-    <t>za_procedure_procedure</t>
   </si>
 </sst>
 </file>
@@ -1202,15 +1199,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E20DF1C-1822-48BD-A5E8-6C607BCB50D4}">
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="75.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="13.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.88671875" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="2"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1363,7 +1360,7 @@
         <v>37051</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>100</v>
@@ -1391,7 +1388,7 @@
         <v>37052</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>100</v>
@@ -1419,7 +1416,7 @@
         <v>37131</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>100</v>
@@ -1475,7 +1472,7 @@
         <v>37171</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>100</v>
@@ -1503,7 +1500,7 @@
         <v>37172</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>100</v>
@@ -1985,7 +1982,7 @@
         <v>197011</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>100</v>
@@ -2036,7 +2033,7 @@
         <v>199906</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>100</v>
@@ -2053,7 +2050,7 @@
         <v>199906</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>100</v>
@@ -2104,7 +2101,7 @@
         <v>199907</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>100</v>
@@ -2121,7 +2118,7 @@
         <v>199907</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>100</v>
@@ -3307,7 +3304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E766E548-8393-46AC-AB7C-3B6B1ADADF6D}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -3945,7 +3942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38C000B-F835-4075-843C-2308CB7B2E7C}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>

</xml_diff>